<commit_message>
change in student table
</commit_message>
<xml_diff>
--- a/Documentation/Database Tables.xlsx
+++ b/Documentation/Database Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP\01 - project chater template\project-charter-template\Documentation\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531495\Desktop\project\project-charter-template\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2EF6CD79-509E-4785-AB0C-A7FB54EF4689}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{55D7CCBF-37D1-4891-8C79-080B4FFEEFD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{E53845C8-7213-4947-BA42-765E622B2AB8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{E53845C8-7213-4947-BA42-765E622B2AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Login Table" sheetId="1" r:id="rId1"/>
@@ -278,9 +278,6 @@
     <t>ALBERT</t>
   </si>
   <si>
-    <t>Cow</t>
-  </si>
-  <si>
     <t>S531493</t>
   </si>
   <si>
@@ -441,6 +438,9 @@
   </si>
   <si>
     <t>Echo</t>
+  </si>
+  <si>
+    <t>Zebra</t>
   </si>
 </sst>
 </file>
@@ -1096,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E3CDB8-F4EF-4525-9D6E-259421BD43A8}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1243,147 +1243,147 @@
         <v>82</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1395,7 +1395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39C0C2B-960B-4D3A-91BF-FFE396B9EE21}">
   <dimension ref="A1:A167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:A184"/>
     </sheetView>
   </sheetViews>
@@ -1406,87 +1406,87 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75">
       <c r="A3" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18.75">
       <c r="A4" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18.75">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18.75">
       <c r="A6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18.75">
       <c r="A7" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18.75">
       <c r="A8" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.75">
       <c r="A9" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.75">
       <c r="A10" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18.75">
       <c r="A11" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18.75">
       <c r="A12" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18.75">
       <c r="A13" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18.75">
       <c r="A14" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18.75">
       <c r="A15" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="18.75">
       <c r="A16" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75">
       <c r="A17" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75">

</xml_diff>